<commit_message>
Edit function for appointments done
</commit_message>
<xml_diff>
--- a/Registru_Programari/excel_database/Registru_programari.xlsx
+++ b/Registru_Programari/excel_database/Registru_programari.xlsx
@@ -7,23 +7,35 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="09-12-2024" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-01-2024" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="04-01-2024" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="03-01-2024" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="02-01-2024" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="31-12-2023" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="30-12-2023" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="29-12-2023" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="05-02-2024" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="22-01-2024" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="15-01-2024" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="12-01-2024" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="10-01-2024" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="09-01-2024" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-01-2024" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="04-01-2024" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="03-01-2024" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="02-01-2024" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="31-12-2023" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="30-12-2023" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="29-12-2023" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'09-12-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'08-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'04-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'03-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'02-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'31-12-2023'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'30-12-2023'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'29-12-2023'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'05-02-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'22-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'15-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'12-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'10-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'09-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'08-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'04-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'03-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'02-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'31-12-2023'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'30-12-2023'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'29-12-2023'!$A$1:$F$17</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -688,7 +700,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -760,26 +772,6 @@
           <t>8:30-9:00</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>MOTAN</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>SFOR SFOR</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>1900106226805</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>0748313432</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="n">
@@ -850,26 +842,6 @@
           <t>13:00-13:30</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>RAZVAN</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>UNGUREANU</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>1900106226805</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>0748313438</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="n">
@@ -908,6 +880,26 @@
       <c r="B14" t="inlineStr">
         <is>
           <t>15:00-15:30</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>RAZVAN</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>UNGUREANU</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>1900106226805</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>0748313438</t>
         </is>
       </c>
     </row>
@@ -947,7 +939,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -962,10 +954,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="21" customWidth="1" min="2" max="2"/>
-    <col width="19" customWidth="1" min="3" max="3"/>
-    <col width="19" customWidth="1" min="4" max="4"/>
-    <col width="23" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="17" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1069,26 +1061,6 @@
           <t>11:00-11:30</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>CRISTIANO</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>RONALDO</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2365478911267</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>0789456123</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="n">
@@ -1137,26 +1109,6 @@
       <c r="B13" t="inlineStr">
         <is>
           <t>14:30-15:00</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>ELENA</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>UNGUREANU</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>1234567892233</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>0741339685</t>
         </is>
       </c>
     </row>
@@ -1206,7 +1158,724 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>ORA</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>PRENUME</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>NUME</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>CNP</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>TELEFON</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>8:00-8:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>8:30-9:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>9:00-9:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>9:30-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10:00-10:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>10:30-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11:00-11:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11:30-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>13:00-13:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>13:30-14:00</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>JEAN</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>VAN DAME</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>8989891123233</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>07514369854</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>14:00-14:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>14:30-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>15:00-15:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>15:30-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>16:00-16:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>16:30-17:00</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F17"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="19" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>ORA</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>PRENUME</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>NUME</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>CNP</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>TELEFON</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>8:00-8:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>8:30-9:00</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>MICHAEL</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>JORDAN</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>5555566666677</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>9:00-9:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>9:30-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10:00-10:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>10:30-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11:00-11:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11:30-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>13:00-13:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>13:30-14:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>14:00-14:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>14:30-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>15:00-15:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>15:30-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>16:00-16:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>16:30-17:00</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F17"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>ORA</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>PRENUME</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>NUME</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>CNP</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>TELEFON</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>8:00-8:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>8:30-9:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>9:00-9:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>9:30-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10:00-10:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>10:30-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11:00-11:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11:30-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>13:00-13:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>13:30-14:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>14:00-14:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>14:30-15:00</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>RAZVAN</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>UNGUREANU</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1900106226805</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>07483134389</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>15:00-15:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>15:30-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>16:00-16:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>16:30-17:00</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F17"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1298,6 +1967,26 @@
           <t>9:30-10:00</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ELENA</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>UNGUREANU</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1234567892233</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>07770232314</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="n">
@@ -1338,26 +2027,6 @@
           <t>11:30-12:00</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>LEO</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>MESSI</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2345612312199</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>07566632143</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="n">
@@ -1408,24 +2077,482 @@
           <t>15:00-15:30</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>RAZVAN</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>UNGUREANU</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>15:30-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>16:00-16:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>16:30-17:00</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F17"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="21" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>ORA</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>PRENUME</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>NUME</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>CNP</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>TELEFON</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>8:00-8:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>8:30-9:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>9:00-9:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>9:30-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10:00-10:30</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>MOTAN PAROS</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>SFORACHEE</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>1900106226805</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0741339685</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>10:30-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11:00-11:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11:30-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>13:00-13:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>13:30-14:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>14:00-14:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>14:30-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>15:00-15:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>15:30-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>16:00-16:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>16:30-17:00</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F17"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="27" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>ORA</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>PRENUME</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>NUME</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>CNP</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>TELEFON</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>8:00-8:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>8:30-9:00</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>IOAN-RAZVAN MOTAN</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">UNGUREANU </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1900106226805</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>0748313438</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>9:00-9:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>9:30-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10:00-10:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>10:30-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11:00-11:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11:30-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>13:00-13:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>13:30-14:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>14:00-14:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>14:30-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>15:00-15:30</t>
         </is>
       </c>
     </row>
@@ -1480,10 +2607,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="21" customWidth="1" min="2" max="2"/>
-    <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="13" customWidth="1" min="5" max="5"/>
-    <col width="17" customWidth="1" min="6" max="6"/>
+    <col width="21" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1577,6 +2704,26 @@
           <t>10:30-11:00</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>GIGI</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>AGOSTIONO</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1112223334449</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0777788899</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="n">
@@ -1607,6 +2754,26 @@
           <t>13:00-13:30</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>IOAN-RAZVAN</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>UNGUREANU</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1900106226805</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0748313438</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="n">
@@ -1645,6 +2812,26 @@
       <c r="B14" t="inlineStr">
         <is>
           <t>15:00-15:30</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>JEAN</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>VALJEAN</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>1123344445566</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>0232444555</t>
         </is>
       </c>
     </row>
@@ -1700,9 +2887,9 @@
   <cols>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
     <col width="23" customWidth="1" min="5" max="5"/>
-    <col width="21" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1816,6 +3003,26 @@
           <t>11:30-12:00</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>PITICUL</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>BARBOS</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1463219871216</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>0232555999</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="n">
@@ -1836,26 +3043,6 @@
           <t>13:30-14:00</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>JEAN</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>VAN DAME</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>8989891123233</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>07514369854</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="n">
@@ -1864,6 +3051,26 @@
       <c r="B12" t="inlineStr">
         <is>
           <t>14:00-14:30</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>PICICA</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>VAMPIR</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2345612345699</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0746213589</t>
         </is>
       </c>
     </row>
@@ -1938,10 +3145,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="21" customWidth="1" min="2" max="2"/>
-    <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="22" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
     <col width="23" customWidth="1" min="5" max="5"/>
-    <col width="19" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1995,26 +3202,6 @@
           <t>8:30-9:00</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>MICHAEL</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>JORDAN</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>5555566666677</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>123456789</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="n">
@@ -2045,6 +3232,26 @@
           <t>10:00-10:30</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>TESTPRENUME</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>NAMETEST</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1111111222222</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0712345678</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="n">
@@ -2083,6 +3290,26 @@
       <c r="B10" t="inlineStr">
         <is>
           <t>13:00-13:30</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>TESTPRENUME2</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>TESTNUME2</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1333334444449</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0232456123</t>
         </is>
       </c>
     </row>
@@ -2174,13 +3401,13 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="19" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
     <col width="23" customWidth="1" min="5" max="5"/>
-    <col width="21" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2324,6 +3551,26 @@
           <t>14:00-14:30</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>MESSI</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>1234567890023</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0789423561</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="n">
@@ -2334,24 +3581,243 @@
           <t>14:30-15:00</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>RAZVAN</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>UNGUREANU</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>1900106226805</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>07483134389</t>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>15:00-15:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>15:30-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>16:00-16:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>16:30-17:00</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F17"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="23" customWidth="1" min="3" max="3"/>
+    <col width="17" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>ORA</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>PRENUME</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>NUME</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>CNP</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>TELEFON</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>8:00-8:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>8:30-9:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>9:00-9:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>9:30-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10:00-10:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>10:30-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11:00-11:30</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CRISTIANO SIU</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>RONALDO</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2365478911267</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0789456115</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11:30-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>13:00-13:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>13:30-14:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>14:00-14:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>14:30-15:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Exe for registru programari
</commit_message>
<xml_diff>
--- a/Registru_Programari/excel_database/Registru_programari.xlsx
+++ b/Registru_Programari/excel_database/Registru_programari.xlsx
@@ -7,63 +7,65 @@
   </bookViews>
   <sheets>
     <sheet name="09-01-2026" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="09-12-2024" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="13-11-2024" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="08-05-2024" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="07-05-2024" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="28-03-2024" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="27-03-2024" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="25-03-2024" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="14-02-2024" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="05-02-2024" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="25-01-2024" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="23-01-2024" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="22-01-2024" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="19-01-2024" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="17-01-2024" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="16-01-2024" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="15-01-2024" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="12-01-2024" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="11-01-2024" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="10-01-2024" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="09-01-2024" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="08-01-2024" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="04-01-2024" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="03-01-2024" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="02-01-2024" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="31-12-2023" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="30-12-2023" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="29-12-2023" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="08-01-2026" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="09-12-2024" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="13-11-2024" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="08-05-2024" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="07-05-2024" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="28-03-2024" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="27-03-2024" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="25-03-2024" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="14-02-2024" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="05-02-2024" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="25-01-2024" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="23-01-2024" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="22-01-2024" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="19-01-2024" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="17-01-2024" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="16-01-2024" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="15-01-2024" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="12-01-2024" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="11-01-2024" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="10-01-2024" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="09-01-2024" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="08-01-2024" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="04-01-2024" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="03-01-2024" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="02-01-2024" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="31-12-2023" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="30-12-2023" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="29-12-2023" sheetId="29" state="visible" r:id="rId29"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'09-01-2026'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'09-12-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'13-11-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'08-05-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'07-05-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'28-03-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'27-03-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'25-03-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'14-02-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'05-02-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'25-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'23-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'22-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'19-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'17-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">'16-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'15-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">'12-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">'11-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">'10-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">'09-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">'08-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">'04-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">'03-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">'02-01-2024'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="25" hidden="1">'31-12-2023'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="26" hidden="1">'30-12-2023'!$A$1:$F$17</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="27" hidden="1">'29-12-2023'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'08-01-2026'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'09-12-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'13-11-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'08-05-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'07-05-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'28-03-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'27-03-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'25-03-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'14-02-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'05-02-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'25-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'23-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'22-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'19-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">'17-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'16-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">'15-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">'12-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">'11-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">'10-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">'09-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">'08-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">'04-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">'03-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="25" hidden="1">'02-01-2024'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="26" hidden="1">'31-12-2023'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="27" hidden="1">'30-12-2023'!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="28" hidden="1">'29-12-2023'!$A$1:$F$17</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -764,9 +766,9 @@
   <cols>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="19" customWidth="1" min="4" max="4"/>
-    <col width="23" customWidth="1" min="5" max="5"/>
-    <col width="21" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="17" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -838,26 +840,6 @@
       <c r="B5" t="inlineStr">
         <is>
           <t>9:30-10:00</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>ELENA</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>UNGUREANU</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1234567892233</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>07770232314</t>
         </is>
       </c>
     </row>
@@ -1005,7 +987,7 @@
     <col width="17" customWidth="1" min="3" max="3"/>
     <col width="19" customWidth="1" min="4" max="4"/>
     <col width="23" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1079,6 +1061,26 @@
           <t>9:30-10:00</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ELENA</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>UNGUREANU</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1234567892233</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>07770232314</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="n">
@@ -1197,26 +1199,6 @@
       <c r="B17" t="inlineStr">
         <is>
           <t>16:30-17:00</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>RAZVAN</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>UNGUREANU</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>1900106226805</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>0748313438</t>
         </is>
       </c>
     </row>
@@ -1242,6 +1224,245 @@
   <cols>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>ORA</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>PRENUME</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>NUME</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>CNP</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>TELEFON</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>8:00-8:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>8:30-9:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>9:00-9:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>9:30-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10:00-10:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>10:30-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11:00-11:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11:30-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>13:00-13:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>13:30-14:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>14:00-14:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>14:30-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>15:00-15:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>15:30-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>16:00-16:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>16:30-17:00</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>RAZVAN</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>UNGUREANU</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>1900106226805</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>0748313438</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F17"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="17" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="23" customWidth="1" min="5" max="5"/>
     <col width="21" customWidth="1" min="6" max="6"/>
@@ -1465,7 +1686,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1704,7 +1925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1943,7 +2164,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2182,7 +2403,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2401,7 +2622,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2640,7 +2861,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2880,225 +3101,6 @@
       <c r="F14" t="inlineStr">
         <is>
           <t>0232444555</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>15:30-16:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>16:00-16:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>16:30-17:00</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:F17"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
-  <cols>
-    <col width="21" customWidth="1" min="2" max="2"/>
-    <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="13" customWidth="1" min="5" max="5"/>
-    <col width="17" customWidth="1" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>ORA</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>PRENUME</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>NUME</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>CNP</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>TELEFON</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>8:00-8:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>8:30-9:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>9:00-9:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>9:30-10:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>10:00-10:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>10:30-11:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>11:00-11:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>11:30-12:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>13:00-13:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>13:30-14:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>14:00-14:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>14:30-15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>15:00-15:30</t>
         </is>
       </c>
     </row>
@@ -3155,8 +3157,8 @@
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="13" customWidth="1" min="5" max="5"/>
-    <col width="17" customWidth="1" min="6" max="6"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3318,6 +3320,26 @@
       <c r="B14" t="inlineStr">
         <is>
           <t>15:00-15:30</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>AAB</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>BBB</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>1234567891112</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>0741339687</t>
         </is>
       </c>
     </row>
@@ -3373,6 +3395,225 @@
   <cols>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="17" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>ORA</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>PRENUME</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>NUME</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>CNP</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>TELEFON</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>8:00-8:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>8:30-9:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>9:00-9:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>9:30-10:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10:00-10:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>10:30-11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>11:00-11:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>11:30-12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>13:00-13:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>13:30-14:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>14:00-14:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>14:30-15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>15:00-15:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>15:30-16:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>16:00-16:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>16:30-17:00</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F17"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="17" customWidth="1" min="3" max="3"/>
     <col width="16" customWidth="1" min="4" max="4"/>
     <col width="23" customWidth="1" min="5" max="5"/>
     <col width="20" customWidth="1" min="6" max="6"/>
@@ -3616,7 +3857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3875,7 +4116,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4114,7 +4355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4353,7 +4594,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4592,7 +4833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4811,7 +5052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5050,7 +5291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5289,7 +5530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5545,8 +5786,8 @@
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="23" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="17" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5708,26 +5949,6 @@
       <c r="B14" t="inlineStr">
         <is>
           <t>15:00-15:30</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>GIGEL</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>GOGU</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>1900106226805</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>0741339685</t>
         </is>
       </c>
     </row>
@@ -5784,8 +6005,8 @@
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="13" customWidth="1" min="5" max="5"/>
-    <col width="17" customWidth="1" min="6" max="6"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5947,6 +6168,26 @@
       <c r="B14" t="inlineStr">
         <is>
           <t>15:00-15:30</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>GIGEL</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>GOGU</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>1900106226805</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>0741339685</t>
         </is>
       </c>
     </row>
@@ -6002,9 +6243,9 @@
   <cols>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="17" customWidth="1" min="4" max="4"/>
-    <col width="23" customWidth="1" min="5" max="5"/>
-    <col width="21" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="17" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6126,26 +6367,6 @@
       <c r="B10" t="inlineStr">
         <is>
           <t>13:00-13:30</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>JEAN</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>CRAIOVA</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>1900120322561</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>07489123451</t>
         </is>
       </c>
     </row>
@@ -6241,9 +6462,9 @@
   <cols>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="13" customWidth="1" min="5" max="5"/>
-    <col width="17" customWidth="1" min="6" max="6"/>
+    <col width="17" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6365,6 +6586,26 @@
       <c r="B10" t="inlineStr">
         <is>
           <t>13:00-13:30</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>JEAN</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>CRAIOVA</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1900120322561</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>07489123451</t>
         </is>
       </c>
     </row>
@@ -6460,9 +6701,9 @@
   <cols>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="16" customWidth="1" min="4" max="4"/>
-    <col width="23" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="17" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6644,26 +6885,6 @@
       <c r="B16" t="inlineStr">
         <is>
           <t>16:00-16:30</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>MICKI</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>VAMPIR</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>1234567891011</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>0712345689</t>
         </is>
       </c>
     </row>
@@ -6699,9 +6920,9 @@
   <cols>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="13" customWidth="1" min="5" max="5"/>
-    <col width="17" customWidth="1" min="6" max="6"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6883,6 +7104,26 @@
       <c r="B16" t="inlineStr">
         <is>
           <t>16:00-16:30</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>MICKI</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>VAMPIR</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>1234567891011</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>0712345689</t>
         </is>
       </c>
     </row>

</xml_diff>